<commit_message>
Changes is made in Reporting and Logging mechanism is added to the framework Signed-off-by: Manish Behera <beheramanishkumar@gmail.com>
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM" sheetId="1" r:id="rId1"/>
+    <sheet name="Population" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -32,14 +33,40 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -412,4 +440,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>